<commit_message>
Sequence_id changed to MEMBER
</commit_message>
<xml_diff>
--- a/test_files/DPM_Metric_Credit.xlsx
+++ b/test_files/DPM_Metric_Credit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21705"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44514071-1687-4278-B2BB-69F5228023FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DD4F187-9CD4-46D4-9729-101FC7938C4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -524,6 +524,9 @@
     <t>Members_600_dpmMetric</t>
   </si>
   <si>
+    <t>MEMBER</t>
+  </si>
+  <si>
     <t>DPMMETRICDATATYPE</t>
   </si>
   <si>
@@ -543,9 +546,6 @@
   </si>
   <si>
     <t>RELATION</t>
-  </si>
-  <si>
-    <t>SEQUENCE_ID</t>
   </si>
   <si>
     <t>Credit</t>
@@ -2701,14 +2701,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
-      <selection activeCell="E2" sqref="E2:E31"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2734,27 +2735,27 @@
         <v>171</v>
       </c>
       <c r="H1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>64</v>
-      </c>
-      <c r="M1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -2766,14 +2767,14 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>173</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>174</v>
       </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
       <c r="H2" t="s">
         <v>26</v>
       </c>
@@ -2781,13 +2782,13 @@
         <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
         <v>163</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="M2" t="s">
         <v>24</v>
@@ -2795,7 +2796,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -2807,14 +2808,14 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>173</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>175</v>
       </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
@@ -2822,13 +2823,13 @@
         <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
         <v>163</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="M3" t="s">
         <v>70</v>
@@ -2836,7 +2837,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -2848,14 +2849,14 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>173</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>176</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
@@ -2863,13 +2864,13 @@
         <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
         <v>163</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="M4" t="s">
         <v>74</v>
@@ -2877,7 +2878,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -2889,14 +2890,14 @@
         <v>26</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>173</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>177</v>
       </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
@@ -2904,13 +2905,13 @@
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
         <v>163</v>
       </c>
       <c r="L5" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="M5" t="s">
         <v>77</v>
@@ -2918,7 +2919,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -2930,14 +2931,14 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>173</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>178</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
@@ -2945,13 +2946,13 @@
         <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
         <v>163</v>
       </c>
       <c r="L6" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="M6" t="s">
         <v>80</v>
@@ -2959,7 +2960,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -2971,14 +2972,14 @@
         <v>26</v>
       </c>
       <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>173</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>179</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
@@ -2986,13 +2987,13 @@
         <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K7" t="s">
         <v>163</v>
       </c>
       <c r="L7" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="M7" t="s">
         <v>83</v>
@@ -3000,7 +3001,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
@@ -3012,14 +3013,14 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
         <v>173</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>180</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
@@ -3027,13 +3028,13 @@
         <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
         <v>163</v>
       </c>
       <c r="L8" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="M8" t="s">
         <v>86</v>
@@ -3041,7 +3042,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -3053,14 +3054,14 @@
         <v>26</v>
       </c>
       <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
         <v>173</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>181</v>
       </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
@@ -3068,13 +3069,13 @@
         <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K9" t="s">
         <v>163</v>
       </c>
       <c r="L9" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="M9" t="s">
         <v>89</v>
@@ -3082,7 +3083,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -3094,14 +3095,14 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
         <v>173</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>182</v>
       </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
@@ -3109,13 +3110,13 @@
         <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
         <v>163</v>
       </c>
       <c r="L10" t="s">
-        <v>92</v>
+        <v>163</v>
       </c>
       <c r="M10" t="s">
         <v>92</v>
@@ -3123,7 +3124,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -3135,14 +3136,14 @@
         <v>26</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
         <v>173</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>183</v>
       </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
@@ -3150,13 +3151,13 @@
         <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K11" t="s">
         <v>163</v>
       </c>
       <c r="L11" t="s">
-        <v>95</v>
+        <v>163</v>
       </c>
       <c r="M11" t="s">
         <v>95</v>
@@ -3164,7 +3165,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3176,14 +3177,14 @@
         <v>26</v>
       </c>
       <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
         <v>173</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>184</v>
       </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
       <c r="H12" t="s">
         <v>26</v>
       </c>
@@ -3191,13 +3192,13 @@
         <v>26</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K12" t="s">
         <v>163</v>
       </c>
       <c r="L12" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="M12" t="s">
         <v>98</v>
@@ -3205,7 +3206,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -3217,14 +3218,14 @@
         <v>26</v>
       </c>
       <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
         <v>173</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>185</v>
       </c>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
@@ -3232,13 +3233,13 @@
         <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K13" t="s">
         <v>163</v>
       </c>
       <c r="L13" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="M13" t="s">
         <v>101</v>
@@ -3246,7 +3247,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -3258,14 +3259,14 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
         <v>173</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>186</v>
       </c>
-      <c r="G14" t="s">
-        <v>26</v>
-      </c>
       <c r="H14" t="s">
         <v>26</v>
       </c>
@@ -3273,13 +3274,13 @@
         <v>26</v>
       </c>
       <c r="J14" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K14" t="s">
         <v>163</v>
       </c>
       <c r="L14" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="M14" t="s">
         <v>104</v>
@@ -3287,7 +3288,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -3299,14 +3300,14 @@
         <v>26</v>
       </c>
       <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
         <v>173</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>187</v>
       </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
       <c r="H15" t="s">
         <v>26</v>
       </c>
@@ -3314,13 +3315,13 @@
         <v>26</v>
       </c>
       <c r="J15" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K15" t="s">
         <v>163</v>
       </c>
       <c r="L15" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
       <c r="M15" t="s">
         <v>107</v>
@@ -3328,7 +3329,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -3340,14 +3341,14 @@
         <v>26</v>
       </c>
       <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
         <v>173</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>188</v>
       </c>
-      <c r="G16" t="s">
-        <v>26</v>
-      </c>
       <c r="H16" t="s">
         <v>26</v>
       </c>
@@ -3355,13 +3356,13 @@
         <v>26</v>
       </c>
       <c r="J16" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K16" t="s">
         <v>163</v>
       </c>
       <c r="L16" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="M16" t="s">
         <v>110</v>
@@ -3369,7 +3370,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -3381,14 +3382,14 @@
         <v>26</v>
       </c>
       <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
         <v>173</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>189</v>
       </c>
-      <c r="G17" t="s">
-        <v>26</v>
-      </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
@@ -3396,13 +3397,13 @@
         <v>26</v>
       </c>
       <c r="J17" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K17" t="s">
         <v>163</v>
       </c>
       <c r="L17" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="M17" t="s">
         <v>113</v>
@@ -3410,7 +3411,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -3422,14 +3423,14 @@
         <v>26</v>
       </c>
       <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
         <v>173</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>190</v>
       </c>
-      <c r="G18" t="s">
-        <v>26</v>
-      </c>
       <c r="H18" t="s">
         <v>26</v>
       </c>
@@ -3437,13 +3438,13 @@
         <v>26</v>
       </c>
       <c r="J18" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K18" t="s">
         <v>163</v>
       </c>
       <c r="L18" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="M18" t="s">
         <v>116</v>
@@ -3451,7 +3452,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -3463,14 +3464,14 @@
         <v>26</v>
       </c>
       <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
         <v>173</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>191</v>
       </c>
-      <c r="G19" t="s">
-        <v>26</v>
-      </c>
       <c r="H19" t="s">
         <v>26</v>
       </c>
@@ -3478,13 +3479,13 @@
         <v>26</v>
       </c>
       <c r="J19" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K19" t="s">
         <v>163</v>
       </c>
       <c r="L19" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="M19" t="s">
         <v>119</v>
@@ -3492,7 +3493,7 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -3504,14 +3505,14 @@
         <v>26</v>
       </c>
       <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
         <v>173</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>192</v>
       </c>
-      <c r="G20" t="s">
-        <v>26</v>
-      </c>
       <c r="H20" t="s">
         <v>26</v>
       </c>
@@ -3519,13 +3520,13 @@
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K20" t="s">
         <v>163</v>
       </c>
       <c r="L20" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="M20" t="s">
         <v>122</v>
@@ -3533,7 +3534,7 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -3545,14 +3546,14 @@
         <v>26</v>
       </c>
       <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
         <v>173</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>193</v>
       </c>
-      <c r="G21" t="s">
-        <v>26</v>
-      </c>
       <c r="H21" t="s">
         <v>26</v>
       </c>
@@ -3560,13 +3561,13 @@
         <v>26</v>
       </c>
       <c r="J21" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K21" t="s">
         <v>163</v>
       </c>
       <c r="L21" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="M21" t="s">
         <v>125</v>
@@ -3574,7 +3575,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
@@ -3586,14 +3587,14 @@
         <v>26</v>
       </c>
       <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
         <v>173</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>194</v>
       </c>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
       <c r="H22" t="s">
         <v>26</v>
       </c>
@@ -3601,13 +3602,13 @@
         <v>26</v>
       </c>
       <c r="J22" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K22" t="s">
         <v>163</v>
       </c>
       <c r="L22" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="M22" t="s">
         <v>128</v>
@@ -3615,7 +3616,7 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -3627,14 +3628,14 @@
         <v>26</v>
       </c>
       <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
         <v>173</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>195</v>
       </c>
-      <c r="G23" t="s">
-        <v>26</v>
-      </c>
       <c r="H23" t="s">
         <v>26</v>
       </c>
@@ -3642,13 +3643,13 @@
         <v>26</v>
       </c>
       <c r="J23" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K23" t="s">
         <v>163</v>
       </c>
       <c r="L23" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="M23" t="s">
         <v>131</v>
@@ -3656,7 +3657,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -3668,14 +3669,14 @@
         <v>26</v>
       </c>
       <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
         <v>173</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>196</v>
       </c>
-      <c r="G24" t="s">
-        <v>26</v>
-      </c>
       <c r="H24" t="s">
         <v>26</v>
       </c>
@@ -3683,13 +3684,13 @@
         <v>26</v>
       </c>
       <c r="J24" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K24" t="s">
         <v>163</v>
       </c>
       <c r="L24" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="M24" t="s">
         <v>134</v>
@@ -3697,7 +3698,7 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -3709,14 +3710,14 @@
         <v>26</v>
       </c>
       <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
         <v>173</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>197</v>
       </c>
-      <c r="G25" t="s">
-        <v>26</v>
-      </c>
       <c r="H25" t="s">
         <v>26</v>
       </c>
@@ -3724,13 +3725,13 @@
         <v>26</v>
       </c>
       <c r="J25" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K25" t="s">
         <v>163</v>
       </c>
       <c r="L25" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="M25" t="s">
         <v>137</v>
@@ -3738,7 +3739,7 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -3750,14 +3751,14 @@
         <v>26</v>
       </c>
       <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
         <v>173</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>198</v>
       </c>
-      <c r="G26" t="s">
-        <v>26</v>
-      </c>
       <c r="H26" t="s">
         <v>26</v>
       </c>
@@ -3765,13 +3766,13 @@
         <v>26</v>
       </c>
       <c r="J26" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K26" t="s">
         <v>163</v>
       </c>
       <c r="L26" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="M26" t="s">
         <v>140</v>
@@ -3779,7 +3780,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -3791,14 +3792,14 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
         <v>173</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>199</v>
       </c>
-      <c r="G27" t="s">
-        <v>26</v>
-      </c>
       <c r="H27" t="s">
         <v>26</v>
       </c>
@@ -3806,13 +3807,13 @@
         <v>26</v>
       </c>
       <c r="J27" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K27" t="s">
         <v>163</v>
       </c>
       <c r="L27" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="M27" t="s">
         <v>143</v>
@@ -3820,7 +3821,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -3832,14 +3833,14 @@
         <v>26</v>
       </c>
       <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
         <v>173</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>200</v>
       </c>
-      <c r="G28" t="s">
-        <v>26</v>
-      </c>
       <c r="H28" t="s">
         <v>26</v>
       </c>
@@ -3847,13 +3848,13 @@
         <v>26</v>
       </c>
       <c r="J28" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K28" t="s">
         <v>163</v>
       </c>
       <c r="L28" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="M28" t="s">
         <v>146</v>
@@ -3861,7 +3862,7 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -3873,14 +3874,14 @@
         <v>26</v>
       </c>
       <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
         <v>173</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>201</v>
       </c>
-      <c r="G29" t="s">
-        <v>26</v>
-      </c>
       <c r="H29" t="s">
         <v>26</v>
       </c>
@@ -3888,13 +3889,13 @@
         <v>26</v>
       </c>
       <c r="J29" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K29" t="s">
         <v>163</v>
       </c>
       <c r="L29" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="M29" t="s">
         <v>149</v>
@@ -3902,7 +3903,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -3914,14 +3915,14 @@
         <v>26</v>
       </c>
       <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
         <v>173</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>202</v>
       </c>
-      <c r="G30" t="s">
-        <v>26</v>
-      </c>
       <c r="H30" t="s">
         <v>26</v>
       </c>
@@ -3929,13 +3930,13 @@
         <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K30" t="s">
         <v>163</v>
       </c>
       <c r="L30" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="M30" t="s">
         <v>152</v>
@@ -3943,7 +3944,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
@@ -3955,14 +3956,14 @@
         <v>26</v>
       </c>
       <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
         <v>173</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>203</v>
       </c>
-      <c r="G31" t="s">
-        <v>26</v>
-      </c>
       <c r="H31" t="s">
         <v>26</v>
       </c>
@@ -3970,13 +3971,13 @@
         <v>26</v>
       </c>
       <c r="J31" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="K31" t="s">
         <v>163</v>
       </c>
       <c r="L31" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="M31" t="s">
         <v>155</v>

</xml_diff>

<commit_message>
MEMBER changed to MEMBER_ID
</commit_message>
<xml_diff>
--- a/test_files/DPM_Metric_Credit.xlsx
+++ b/test_files/DPM_Metric_Credit.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21705"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DD4F187-9CD4-46D4-9729-101FC7938C4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17CD74B0-025F-40A6-9B4E-96547BBA0A79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
     <t>Members_600_dpmMetric</t>
   </si>
   <si>
-    <t>MEMBER</t>
+    <t>MEMBER_ID</t>
   </si>
   <si>
     <t>DPMMETRICDATATYPE</t>
@@ -2702,7 +2702,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>